<commit_message>
Upload Employee Bug Fixed
</commit_message>
<xml_diff>
--- a/spectoProject/configuration/handle_uploaded_file/Employees.xlsx
+++ b/spectoProject/configuration/handle_uploaded_file/Employees.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\dev\frontend\venvSpecto\specto\spectoProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765B2D2D-57B2-4391-9F27-09DA65B7DC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2428A60C-8AF4-4714-BC40-E8166C22C500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Mat</t>
   </si>
@@ -69,12 +81,6 @@
     <t>Matricule Resp. Fab N+2</t>
   </si>
   <si>
-    <t>Resp. Fab N+2</t>
-  </si>
-  <si>
-    <t>TABLEAU EFFECTIF AFS</t>
-  </si>
-  <si>
     <t>SELMI  Houssem Edine</t>
   </si>
   <si>
@@ -99,7 +105,1874 @@
     <t>MATOUSSI SALAH</t>
   </si>
   <si>
-    <t>KARIM  MLAIKI</t>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>matricule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IntegerField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>unique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>names</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>i_p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>department</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ForeignKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>on_delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CASCADE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ForeignKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>on_delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CASCADE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>workshop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ForeignKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Workshop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>on_delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CASCADE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>wording</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cost_center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>job_bulletin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>resp_matricule_n1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IntegerField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>resp_names_n1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>resp_matricule_n2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IntegerField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>resp_names_n2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>staff_tab_afs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>max_length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>employee.</t>
   </si>
 </sst>
 </file>
@@ -109,7 +1982,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +2001,49 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFE06C75"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF56B6C2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFE5C07B"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FFE06C75"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD19A66"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF61AFEF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,7 +2122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,6 +2153,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +2463,7 @@
     <col min="16" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,31 +2506,27 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>81780</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="9">
         <v>0</v>
@@ -620,31 +2535,239 @@
         <v>0</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="L2" s="8">
         <v>82151</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N2" s="8">
         <v>81813</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B3EF81-4203-42FC-A3E8-05E06B1944C3}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A1&amp;B1</f>
+        <v>employee.    matricule = models.IntegerField(unique=True)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C16" si="0">A2&amp;B2</f>
+        <v>employee.    names = models.CharField(max_length= 100)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    i_p = models.CharField(max_length=2)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    code = models.CharField(max_length=50)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    department = models.CharField(max_length=50)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    program = models.ForeignKey(Program,on_delete=models.CASCADE)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    product = models.ForeignKey(Product,on_delete=models.CASCADE)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    workshop = models.ForeignKey(Workshop,on_delete=models.CASCADE)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    wording = models.CharField(max_length=100)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    cost_center = models.CharField(max_length=30)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    job_bulletin = models.CharField(max_length=100)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    resp_matricule_n1 = models.IntegerField()</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    resp_names_n1 = models.CharField(max_length=100)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    resp_matricule_n2 = models.IntegerField()</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    resp_names_n2 = models.CharField(max_length=100)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>employee.    staff_tab_afs = models.CharField(max_length=50)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>